<commit_message>
Updated backend and frontend functionality with recent changes
</commit_message>
<xml_diff>
--- a/customer_requests.xlsx
+++ b/customer_requests.xlsx
@@ -2,16 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4200" yWindow="500" windowWidth="29400" windowHeight="18980" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Requests" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Billing" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -51,7 +50,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -414,13 +413,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -452,22 +451,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SHREE</t>
+          <t>ds</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2000</t>
+          <t>5675</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024-09-06</t>
+          <t>2024-09-10</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2024-09-20</t>
+          <t>2024-09-12</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -479,22 +478,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SHREE</t>
+          <t>ds</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>5667</t>
+          <t>34243</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2024-09-06</t>
+          <t>2024-09-20</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-27</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -506,108 +505,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>hg</t>
+          <t>SHREE</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5000</t>
+          <t>677</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2024-09-04</t>
+          <t>2024-09-10</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2024-09-20</t>
+          <t>2024-09-19</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
           <t>Yes</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>ds</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>5454</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2024-09-06</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2024-09-20</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>ds</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>6565</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2024-09-06</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2024-09-19</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>SHREE</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>20000</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>2024-09-07</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>2024-09-27</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>No</t>
         </is>
       </c>
     </row>
@@ -622,13 +540,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -654,6 +572,50 @@
       <c r="E1" t="inlineStr">
         <is>
           <t>Status</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>hgd</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>3244423</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2024-09-26</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ds</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>34243</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2024-09-20</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2024-09-27</t>
         </is>
       </c>
     </row>

</xml_diff>